<commit_message>
Created draft GANTT chart, finished planning section, need to finish scientific products section.
</commit_message>
<xml_diff>
--- a/plans/gantt-chart.xlsx
+++ b/plans/gantt-chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81928EA4-3863-4ACA-BADE-1D1912B7D17C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671CC11E-4D57-48FC-A023-D03B5FA41FCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Year 1</t>
   </si>
@@ -40,26 +40,71 @@
     <t>Year 2</t>
   </si>
   <si>
-    <t>Research Planned</t>
-  </si>
-  <si>
-    <t>Administrative Work</t>
-  </si>
-  <si>
-    <t>Primary Scientific Results</t>
-  </si>
-  <si>
-    <t>Secondary Scientific Results</t>
-  </si>
-  <si>
     <t>Year 3</t>
+  </si>
+  <si>
+    <t>WP1</t>
+  </si>
+  <si>
+    <t>WP2</t>
+  </si>
+  <si>
+    <t>WP3</t>
+  </si>
+  <si>
+    <t>WP4</t>
+  </si>
+  <si>
+    <t>Publication of Paper 2</t>
+  </si>
+  <si>
+    <t>Publication of Paper 1</t>
+  </si>
+  <si>
+    <t>Publication of Paper 4</t>
+  </si>
+  <si>
+    <t>Publication of Paper 3</t>
+  </si>
+  <si>
+    <t>T4.3: Apply PySPAM</t>
+  </si>
+  <si>
+    <t>T4.2: Parametric Analysis</t>
+  </si>
+  <si>
+    <t>T4.1: Interacting Galaxy Selection</t>
+  </si>
+  <si>
+    <t>T3.3: Matching to published catalogue</t>
+  </si>
+  <si>
+    <t>T3.2: Building Code for Parametric Analysis</t>
+  </si>
+  <si>
+    <t>T3.1: Acquinting self with Eucid Data</t>
+  </si>
+  <si>
+    <t>T1.2: Building Training Set</t>
+  </si>
+  <si>
+    <t>T1.1: Building Pipeline</t>
+  </si>
+  <si>
+    <t>T1.3: Diagnostics of Zoobot</t>
+  </si>
+  <si>
+    <t>T2.1: Matching to existing catalogues</t>
+  </si>
+  <si>
+    <t>T2.2: Building Code for Analysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,16 +112,77 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -128,15 +234,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -183,11 +280,408 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,69 +698,210 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="31" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="36" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="5" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -544,23 +1179,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P7"/>
+  <dimension ref="B1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="13.6328125" customWidth="1"/>
-    <col min="4" max="7" width="8.7265625" style="2"/>
-    <col min="8" max="16" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="18.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.08984375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.08984375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.36328125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
+    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
@@ -574,135 +1220,278 @@
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
       <c r="L2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="25"/>
+    <row r="4" spans="2:15" ht="54.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="21"/>
     </row>
     <row r="5" spans="2:15" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="25"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="21"/>
     </row>
     <row r="6" spans="2:15" ht="48.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="46"/>
+      <c r="C6" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="21"/>
+    </row>
+    <row r="7" spans="2:15" ht="51.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="25"/>
+      <c r="C7" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="21"/>
     </row>
-    <row r="7" spans="2:15" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="16" t="s">
+    <row r="8" spans="2:15" ht="57.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="45"/>
+      <c r="C8" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="21"/>
+    </row>
+    <row r="9" spans="2:15" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="25"/>
+      <c r="C9" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" spans="2:15" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="48"/>
+      <c r="C10" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="67"/>
+    </row>
+    <row r="11" spans="2:15" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="49"/>
+      <c r="C11" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="68"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="21"/>
+    </row>
+    <row r="12" spans="2:15" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="35"/>
+    </row>
+    <row r="13" spans="2:15" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="51"/>
+      <c r="C13" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="61"/>
+    </row>
+    <row r="14" spans="2:15" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="52"/>
+      <c r="C14" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="44" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalised proposal documents, sent of to referees and finalised GANTT chart. Waiting for Sandor to get back to me, and we are a go!
</commit_message>
<xml_diff>
--- a/plans/gantt-chart.xlsx
+++ b/plans/gantt-chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA26672-326B-4A34-A5AE-DCCF9ABE6CAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6994F35D-A336-40E1-A374-17AC797452D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,20 +98,20 @@
     <t>R3: Release of Combined Catalogue and Initial Analysis</t>
   </si>
   <si>
-    <t>D2: A Spectroscopically Confirmed Catalogue of Interacting Galaxies</t>
-  </si>
-  <si>
-    <t>R4: Analysis of Interacting Galaxy Catalogue and Exploration of Parameter Space Linking AGN and Interaction</t>
-  </si>
-  <si>
-    <t>D1: Repository of 3-Colour Cutouts for Entire JWST and Hubble Public Archives</t>
+    <t>D1: Repository rest frame images in HST and JWST archives</t>
+  </si>
+  <si>
+    <t>D2: Spectroscopically Confirmed Catalogue of Interacting Galaxies</t>
+  </si>
+  <si>
+    <t>R4: Analysis of Interacting Galaxy Catalogue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,42 +156,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -711,7 +705,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -810,6 +804,33 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,113 +843,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1217,104 +1217,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.6328125" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.6328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.08984375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.90625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.08984375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="27.6328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7265625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27.36328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="27.453125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="25.6328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="27.54296875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="27.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.90625" customWidth="1"/>
+    <col min="4" max="4" width="36.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.08984375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="36.90625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="36.7265625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="37" style="1" customWidth="1"/>
+    <col min="10" max="11" width="36.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="39.6328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="36.26953125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="37.6328125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="40.6328125" style="1" customWidth="1"/>
     <col min="16" max="16" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="56" t="s">
+    <row r="2" spans="2:15" ht="36.5" thickBot="1" x14ac:dyDescent="0.85">
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="56" t="s">
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="56" t="s">
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="58"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="75"/>
     </row>
-    <row r="3" spans="2:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="54" t="s">
+    <row r="3" spans="2:15" ht="36.5" thickBot="1" x14ac:dyDescent="0.85">
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="55" t="s">
+      <c r="I3" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="55" t="s">
+      <c r="L3" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="55" t="s">
+      <c r="M3" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="55" t="s">
+      <c r="N3" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="55" t="s">
+      <c r="O3" s="72" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="105.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="38" t="s">
+    <row r="4" spans="2:15" ht="151" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="58" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="61" t="s">
-        <v>27</v>
+      <c r="G4" s="69" t="s">
+        <v>25</v>
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="17"/>
@@ -1325,9 +1323,9 @@
       <c r="N4" s="15"/>
       <c r="O4" s="7"/>
     </row>
-    <row r="5" spans="2:15" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="39"/>
-      <c r="C5" s="51" t="s">
+    <row r="5" spans="2:15" ht="151" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="51"/>
+      <c r="C5" s="58" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="9"/>
@@ -1343,16 +1341,16 @@
       <c r="N5" s="17"/>
       <c r="O5" s="7"/>
     </row>
-    <row r="6" spans="2:15" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="40"/>
-      <c r="C6" s="52" t="s">
+    <row r="6" spans="2:15" ht="148.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="52"/>
+      <c r="C6" s="59" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="12"/>
       <c r="F6" s="11"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="65" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="17"/>
@@ -1363,18 +1361,18 @@
       <c r="N6" s="15"/>
       <c r="O6" s="7"/>
     </row>
-    <row r="7" spans="2:15" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="2:15" ht="152.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="61" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="62"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="68"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
       <c r="K7" s="32"/>
@@ -1383,17 +1381,17 @@
       <c r="N7" s="17"/>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="2:15" ht="101.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="48"/>
-      <c r="C8" s="49" t="s">
+    <row r="8" spans="2:15" ht="158" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="54"/>
+      <c r="C8" s="60" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="12"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="70"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="15"/>
       <c r="K8" s="7"/>
       <c r="L8" s="15"/>
@@ -1401,18 +1399,18 @@
       <c r="N8" s="15"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="2:15" ht="106.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="42"/>
-      <c r="C9" s="49" t="s">
+    <row r="9" spans="2:15" ht="156" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="55"/>
+      <c r="C9" s="61" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
       <c r="F9" s="17"/>
       <c r="G9" s="33"/>
-      <c r="H9" s="69"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="20"/>
-      <c r="J9" s="65" t="s">
+      <c r="J9" s="66" t="s">
         <v>23</v>
       </c>
       <c r="K9" s="7"/>
@@ -1421,39 +1419,39 @@
       <c r="N9" s="15"/>
       <c r="O9" s="7"/>
     </row>
-    <row r="10" spans="2:15" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="43" t="s">
+    <row r="10" spans="2:15" ht="151" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="63" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="73"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="16"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="7"/>
     </row>
-    <row r="11" spans="2:15" ht="101.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="44"/>
-      <c r="C11" s="50" t="s">
+    <row r="11" spans="2:15" ht="148" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="57"/>
+      <c r="C11" s="62" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="59"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="21"/>
       <c r="J11" s="22"/>
-      <c r="K11" s="66" t="s">
+      <c r="K11" s="67" t="s">
         <v>24</v>
       </c>
       <c r="L11" s="30"/>
@@ -1461,11 +1459,11 @@
       <c r="N11" s="31"/>
       <c r="O11" s="32"/>
     </row>
-    <row r="12" spans="2:15" ht="102.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="45" t="s">
+    <row r="12" spans="2:15" ht="151.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="64" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="16"/>
@@ -1476,16 +1474,16 @@
       <c r="I12" s="3"/>
       <c r="J12" s="23"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="63" t="s">
-        <v>25</v>
+      <c r="L12" s="68" t="s">
+        <v>26</v>
       </c>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="19"/>
     </row>
-    <row r="13" spans="2:15" ht="105.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="46"/>
-      <c r="C13" s="53" t="s">
+    <row r="13" spans="2:15" ht="149" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="48"/>
+      <c r="C13" s="64" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="16"/>
@@ -1501,9 +1499,9 @@
       <c r="N13" s="3"/>
       <c r="O13" s="28"/>
     </row>
-    <row r="14" spans="2:15" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="47"/>
-      <c r="C14" s="53" t="s">
+    <row r="14" spans="2:15" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="49"/>
+      <c r="C14" s="64" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="16"/>
@@ -1517,20 +1515,20 @@
       <c r="L14" s="29"/>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
-      <c r="O14" s="64" t="s">
-        <v>26</v>
+      <c r="O14" s="70" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:K2"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>